<commit_message>
update to output folder
</commit_message>
<xml_diff>
--- a/docs/template-basic.xlsx
+++ b/docs/template-basic.xlsx
@@ -151,7 +151,7 @@
   </si>
   <si>
     <t>dom-2:If the resource is contained in another resource, it SHALL NOT contain nested Resources {contained.contained.empty()}
-dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.all(('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists())}temp-1:Identifier SHALL be greater than 5 characters {Identifier.value.length()&gt;5}</t>
+dom-1:If the resource is contained in another resource, it SHALL NOT contain any narrative {contained.text.empty()}dom-4:If a resource is contained in another resource, it SHALL NOT have a meta.versionId or a meta.lastUpdated {contained.meta.versionId.empty() and contained.meta.lastUpdated.empty()}dom-3:If the resource is contained in another resource, it SHALL be referred to from elsewhere in the resource or SHALL refer to the containing resource {contained.where((('#'+id in (%resource.descendants().reference | %resource.descendants().as(canonical))) or descendants().where(reference = '#').exists() or descendants().where(as(canonical) = '#').exists()).not()).trace('unmatched', id).empty()}dom-6:A resource should have narrative for robust management {text.div.exists()}dom-5:If a resource is contained in another resource, it SHALL NOT have a security label {contained.meta.security.empty()}temp-1:Identifier SHALL be greater than 5 characters {Identifier.value.length()&gt;5}</t>
   </si>
   <si>
     <t>Act, Entity or Role</t>
@@ -292,7 +292,7 @@
     <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
   </si>
   <si>
-    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again.</t>
+    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL not have security labels.</t>
   </si>
   <si>
     <t>DomainResource.contained</t>

</xml_diff>

<commit_message>
update to demonstrate ig pub render error
</commit_message>
<xml_diff>
--- a/docs/template-basic.xlsx
+++ b/docs/template-basic.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$41</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="277">
   <si>
     <t>Path</t>
   </si>
@@ -233,7 +233,7 @@
     <t>Language is provided to support indexing and accessibility (typically, services such as text to speech use the language tag). The html language tag in the narrative applies  to the narrative. The language tag on the resource may be used to specify the language of other presentations generated from the data in the resource. Not all the content has to be in the base language. The Resource.language should not be assumed to apply to the narrative automatically. If a language is specified, it should it also be specified on the div element in the html (see rules in HTML5 for information about the relationship between xml:lang and the html lang attribute).</t>
   </si>
   <si>
-    <t>extensible</t>
+    <t>preferred</t>
   </si>
   <si>
     <t>A human language.</t>
@@ -262,7 +262,7 @@
     <t>A human-readable narrative that contains a summary of the resource and can be used to represent the content of the resource to a human. The narrative need not encode all the structured data, but is required to contain sufficient detail to make it "clinically safe" for a human to just read the narrative. Resource definitions may define what content should be represented in the narrative to ensure clinical safety.</t>
   </si>
   <si>
-    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded in formation is added later.</t>
+    <t>Contained resources do not have narrative. Resources that are not contained SHOULD have a narrative. In some cases, a resource may only have text with little or no additional discrete data (as long as all minOccurs=1 elements are satisfied).  This may be necessary for data from legacy systems where information is captured as a "text blob" or where text is additionally entered raw or narrated and encoded information is added later.</t>
   </si>
   <si>
     <t>DomainResource.text</t>
@@ -288,7 +288,7 @@
     <t>These resources do not have an independent existence apart from the resource that contains them - they cannot be identified independently, and nor can they have their own independent transaction scope.</t>
   </si>
   <si>
-    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL not have security labels.</t>
+    <t>This should never be done when the content can be identified properly, as once identification is lost, it is extremely difficult (and context dependent) to restore it again. Contained resources may have profiles and tags In their meta elements, but SHALL NOT have security labels.</t>
   </si>
   <si>
     <t>DomainResource.contained</t>
@@ -364,7 +364,8 @@
     <t>Extensions that cannot be ignored</t>
   </si>
   <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.</t>
+    <t>May be used to represent additional information that is not part of the basic definition of the resource, and that modifies the understanding of the element that contains it. Usually modifier elements provide negation or qualification. To make the use of extensions safe and manageable, there is a strict set of governance applied to the definition and use of extensions. Though any implementer is allowed to define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension. Applications processing a resource are required to check for modifier extensions.
+Modifier extensions SHALL NOT change the meaning of any elements on Resource or DomainResource (including cannot change the meaning of modifierExtension itself).</t>
   </si>
   <si>
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
@@ -392,13 +393,238 @@
     <t>FiveWs.identifier</t>
   </si>
   <si>
-    <t>Basic.code</t>
+    <t>Basic.identifier.id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">string {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>xml:id (or equivalent in JSON)</t>
+  </si>
+  <si>
+    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
+  </si>
+  <si>
+    <t>Element.id</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Basic.identifier.extension</t>
+  </si>
+  <si>
+    <t>Additional content defined by implementations</t>
+  </si>
+  <si>
+    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
+  </si>
+  <si>
+    <t>Extensions are always sliced by (at least) url</t>
+  </si>
+  <si>
+    <t>Element.extension</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extension {[CanonicalType[http://www.fhir.org/guides/test3/StructureDefinition/extension-identifier-status]]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Basic.identifier.extension.id</t>
+  </si>
+  <si>
+    <t>Basic.identifier.extension.extension</t>
+  </si>
+  <si>
+    <t>Basic.identifier.extension.url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">null {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>identifies the meaning of the extension</t>
+  </si>
+  <si>
+    <t>Source of the definition for the extension code - a logical name or a URL.</t>
+  </si>
+  <si>
+    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
+  </si>
+  <si>
+    <t>Extension.url</t>
+  </si>
+  <si>
+    <t>Basic.identifier.extension.value[x]</t>
+  </si>
+  <si>
+    <t>base64Binary {[]} {[]}
+boolean {[]} {[]}canonical {[]} {[]}code {[]} {[]}date {[]} {[]}dateTime {[]} {[]}decimal {[]} {[]}id {[]} {[]}instant {[]} {[]}integer {[]} {[]}markdown {[]} {[]}oid {[]} {[]}positiveInt {[]} {[]}string {[]} {[]}time {[]} {[]}unsignedInt {[]} {[]}uri {[]} {[]}url {[]} {[]}uuid {[]} {[]}Address {[]} {[]}Age {[]} {[]}Annotation {[]} {[]}Attachment {[]} {[]}CodeableConcept {[]} {[]}Coding {[]} {[]}ContactPoint {[]} {[]}Count {[]} {[]}Distance {[]} {[]}Duration {[]} {[]}HumanName {[]} {[]}Identifier {[]} {[]}Money {[]} {[]}Period {[]} {[]}Quantity {[]} {[]}Range {[]} {[]}Ratio {[]} {[]}Reference {[]} {[]}SampledData {[]} {[]}Signature {[]} {[]}Timing {[]} {[]}ParameterDefinition {[]} {[]}DataRequirement {[]} {[]}RelatedArtifact {[]} {[]}ContactDetail {[]} {[]}Contributor {[]} {[]}TriggerDefinition {[]} {[]}Expression {[]} {[]}UsageContext {[]} {[]}Dosage {[]} {[]}</t>
+  </si>
+  <si>
+    <t>Value of extension</t>
+  </si>
+  <si>
+    <t>Value of extension - may be a resource or one of a constrained set of the data types (see Extensibility in the spec for list).</t>
+  </si>
+  <si>
+    <t>Extension.value[x]</t>
+  </si>
+  <si>
+    <t>Basic.identifier.use</t>
+  </si>
+  <si>
+    <t>usual | official | temp | secondary | old (If known)</t>
+  </si>
+  <si>
+    <t>The purpose of this identifier.</t>
+  </si>
+  <si>
+    <t>Applications can assume that an identifier is permanent unless it explicitly says that it is temporary.</t>
+  </si>
+  <si>
+    <t>Allows the appropriate identifier for a particular context of use to be selected from among a set of identifiers.</t>
+  </si>
+  <si>
+    <t>required</t>
+  </si>
+  <si>
+    <t>Identifies the purpose for this identifier, if known .</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/identifier-use</t>
+  </si>
+  <si>
+    <t>Identifier.use</t>
+  </si>
+  <si>
+    <t>Role.code or implied by context</t>
+  </si>
+  <si>
+    <t>Basic.identifier.type</t>
   </si>
   <si>
     <t xml:space="preserve">CodeableConcept {[]} {[]}
 </t>
   </si>
   <si>
+    <t>Description of identifier</t>
+  </si>
+  <si>
+    <t>A coded type for the identifier that can be used to determine which identifier to use for a specific purpose.</t>
+  </si>
+  <si>
+    <t>This element deals only with general categories of identifiers.  It SHOULD not be used for codes that correspond 1..1 with the Identifier.system. Some identifiers may fall into multiple categories due to common usage.   Where the system is known, a type is unnecessary because the type is always part of the system definition. However systems often need to handle identifiers where the system is not known. There is not a 1:1 relationship between type and system, since many different systems have the same type.</t>
+  </si>
+  <si>
+    <t>Allows users to make use of identifiers when the identifier system is not known.</t>
+  </si>
+  <si>
+    <t>extensible</t>
+  </si>
+  <si>
+    <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
+  </si>
+  <si>
+    <t>Identifier.type</t>
+  </si>
+  <si>
+    <t>Basic.identifier.system</t>
+  </si>
+  <si>
+    <t>The namespace for the identifier value</t>
+  </si>
+  <si>
+    <t>Establishes the namespace for the value - that is, a URL that describes a set values that are unique.</t>
+  </si>
+  <si>
+    <t>Identifier.system is always case sensitive.</t>
+  </si>
+  <si>
+    <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
+  </si>
+  <si>
+    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://www.acme.com/identifiers/patient"/&gt;</t>
+  </si>
+  <si>
+    <t>Identifier.system</t>
+  </si>
+  <si>
+    <t>II.root or Role.id.root</t>
+  </si>
+  <si>
+    <t>Basic.identifier.value</t>
+  </si>
+  <si>
+    <t>The value that is unique</t>
+  </si>
+  <si>
+    <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
+  </si>
+  <si>
+    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
+  </si>
+  <si>
+    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="123456"/&gt;</t>
+  </si>
+  <si>
+    <t>Identifier.value</t>
+  </si>
+  <si>
+    <t>II.extension or II.root if system indicates OID or GUID (Or Role.id.extension or root)</t>
+  </si>
+  <si>
+    <t>Basic.identifier.period</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Period {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Time period when id is/was valid for use</t>
+  </si>
+  <si>
+    <t>Time period during which identifier is/was valid for use.</t>
+  </si>
+  <si>
+    <t>Identifier.period</t>
+  </si>
+  <si>
+    <t>Role.effectiveTime or implied by context</t>
+  </si>
+  <si>
+    <t>Basic.identifier.assigner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]}
+</t>
+  </si>
+  <si>
+    <t>Organization that issued id (may be just text)</t>
+  </si>
+  <si>
+    <t>Organization that issued/manages the identifier.</t>
+  </si>
+  <si>
+    <t>The Identifier.assigner may omit the .reference element and only contain a .display element reflecting the name or other textual information about the assigning organization.</t>
+  </si>
+  <si>
+    <t>Identifier.assigner</t>
+  </si>
+  <si>
+    <t>II.assigningAuthorityName but note that this is an improper use by the definition of the field.  Also Role.scoper</t>
+  </si>
+  <si>
+    <t>Basic.code</t>
+  </si>
+  <si>
     <t>Kind of Resource</t>
   </si>
   <si>
@@ -415,7 +641,7 @@
     <t>example</t>
   </si>
   <si>
-    <t>Codes for identifying types of resources not yet defined by FHIR</t>
+    <t>Codes for identifying types of resources not yet defined by FHIR.</t>
   </si>
   <si>
     <t>http://hl7.org/fhir/ValueSet/basic-resource-type</t>
@@ -430,35 +656,7 @@
     <t>Basic.code.id</t>
   </si>
   <si>
-    <t xml:space="preserve">string {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>xml:id (or equivalent in JSON)</t>
-  </si>
-  <si>
-    <t>Unique id for the element within a resource (for internal references). This may be any string value that does not contain spaces.</t>
-  </si>
-  <si>
-    <t>Element.id</t>
-  </si>
-  <si>
-    <t>n/a</t>
-  </si>
-  <si>
     <t>Basic.code.extension</t>
-  </si>
-  <si>
-    <t>Additional content defined by implementations</t>
-  </si>
-  <si>
-    <t>May be used to represent additional information that is not part of the basic definition of the element. To make the use of extensions safe and manageable, there is a strict set of governance  applied to the definition and use of extensions. Though any implementer can define an extension, there is a set of requirements that SHALL be met as part of the definition of the extension.</t>
-  </si>
-  <si>
-    <t>Extensions are always sliced by (at least) url</t>
-  </si>
-  <si>
-    <t>Element.extension</t>
   </si>
   <si>
     <t>Basic.code.coding</t>
@@ -477,7 +675,7 @@
     <t>Codes may be defined very casually in enumerations, or code lists, up to very formal definitions such as SNOMED CT - see the HL7 v3 Core Principles for more information.  Ordering of codings is undefined and SHALL NOT be used to infer meaning. Generally, at most only one of the coding values will be labeled as UserSelected = true.</t>
   </si>
   <si>
-    <t>Allows for translations and alternate encodings within a code system.  Also supports communication of the same instance to systems requiring different encodings.</t>
+    <t>Allows for alternative encodings within a code system, and translations to other code systems.</t>
   </si>
   <si>
     <t>CodeableConcept.coding</t>
@@ -577,7 +775,7 @@
     <t>If this coding was chosen directly by the user</t>
   </si>
   <si>
-    <t>Indicates that this coding was chosen by a user directly - i.e. off a pick list of available items (codes or displays).</t>
+    <t>Indicates that this coding was chosen by a user directly - e.g. off a pick list of available items (codes or displays).</t>
   </si>
   <si>
     <t>Amongst a set of alternatives, a directly chosen code is the most appropriate starting point for new translations. There is some ambiguity about what exactly 'directly chosen' implies, and trading partner agreement may be needed to clarify the use of this element and its consequences more completely.</t>
@@ -828,7 +1026,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AL28"/>
+  <dimension ref="A1:AL41"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -837,7 +1035,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="29.99609375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="34.30859375" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="19.39453125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="40.90625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
@@ -860,7 +1058,7 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="62.0078125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="101.46875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="48.296875" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
@@ -872,7 +1070,7 @@
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="75.62109375" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="106.1796875" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="24.26171875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2249,7 +2447,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>47</v>
@@ -2258,10 +2456,10 @@
         <v>41</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J14" t="s" s="2">
         <v>120</v>
@@ -2272,12 +2470,8 @@
       <c r="L14" t="s" s="2">
         <v>122</v>
       </c>
-      <c r="M14" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="N14" t="s" s="2">
-        <v>124</v>
-      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
       <c r="O14" t="s" s="2">
         <v>41</v>
       </c>
@@ -2301,13 +2495,13 @@
         <v>41</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>126</v>
+        <v>41</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>127</v>
+        <v>41</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>41</v>
@@ -2325,10 +2519,10 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>47</v>
@@ -2340,26 +2534,26 @@
         <v>41</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>129</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>41</v>
@@ -2371,15 +2565,17 @@
         <v>41</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M15" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="M15" t="s" s="2">
+        <v>111</v>
+      </c>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>41</v>
@@ -2416,25 +2612,25 @@
         <v>41</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="AC15" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>41</v>
@@ -2443,29 +2639,31 @@
         <v>41</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="16" hidden="true">
+    <row r="16">
       <c r="A16" t="s" s="2">
-        <v>136</v>
-      </c>
-      <c r="B16" s="2"/>
+        <v>125</v>
+      </c>
+      <c r="B16" t="s" s="2">
+        <v>130</v>
+      </c>
       <c r="C16" t="s" s="2">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>41</v>
@@ -2474,17 +2672,15 @@
         <v>41</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>91</v>
+        <v>131</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>137</v>
+        <v>92</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>138</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>111</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
         <v>41</v>
@@ -2521,19 +2717,19 @@
         <v>41</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>139</v>
+        <v>41</v>
       </c>
       <c r="AC16" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>140</v>
+        <v>129</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>39</v>
@@ -2548,15 +2744,15 @@
         <v>41</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>135</v>
+        <v>41</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2564,35 +2760,31 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="M17" t="s" s="2">
-        <v>145</v>
-      </c>
-      <c r="N17" t="s" s="2">
-        <v>146</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
       <c r="O17" t="s" s="2">
         <v>41</v>
       </c>
@@ -2640,13 +2832,13 @@
         <v>41</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>41</v>
@@ -2655,7 +2847,7 @@
         <v>41</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>41</v>
@@ -2663,18 +2855,18 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>41</v>
@@ -2686,15 +2878,17 @@
         <v>41</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>133</v>
-      </c>
-      <c r="M18" s="2"/>
+        <v>127</v>
+      </c>
+      <c r="M18" t="s" s="2">
+        <v>111</v>
+      </c>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
         <v>41</v>
@@ -2731,25 +2925,25 @@
         <v>41</v>
       </c>
       <c r="AA18" t="s" s="2">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="AB18" t="s" s="2">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="AC18" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD18" t="s" s="2">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>41</v>
@@ -2758,7 +2952,7 @@
         <v>41</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>41</v>
@@ -2766,18 +2960,18 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>41</v>
@@ -2789,16 +2983,16 @@
         <v>41</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="K19" t="s" s="2">
+        <v>136</v>
+      </c>
+      <c r="L19" t="s" s="2">
         <v>137</v>
       </c>
-      <c r="L19" t="s" s="2">
+      <c r="M19" t="s" s="2">
         <v>138</v>
-      </c>
-      <c r="M19" t="s" s="2">
-        <v>111</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -2836,25 +3030,25 @@
         <v>41</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="AB19" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC19" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD19" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE19" t="s" s="2">
         <v>139</v>
       </c>
-      <c r="AC19" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD19" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AE19" t="s" s="2">
-        <v>140</v>
-      </c>
       <c r="AF19" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>41</v>
@@ -2863,7 +3057,7 @@
         <v>41</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>135</v>
+        <v>89</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>41</v>
@@ -2871,7 +3065,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>151</v>
+        <v>140</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -2891,23 +3085,19 @@
         <v>41</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>60</v>
+        <v>141</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>153</v>
-      </c>
-      <c r="M20" t="s" s="2">
-        <v>154</v>
-      </c>
-      <c r="N20" t="s" s="2">
-        <v>155</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
       <c r="O20" t="s" s="2">
         <v>41</v>
       </c>
@@ -2955,7 +3145,7 @@
         <v>41</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -2970,7 +3160,7 @@
         <v>41</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>157</v>
+        <v>89</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>41</v>
@@ -2978,7 +3168,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -2995,24 +3185,26 @@
         <v>41</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>131</v>
+        <v>66</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>161</v>
-      </c>
-      <c r="N21" s="2"/>
+        <v>148</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>149</v>
+      </c>
       <c r="O21" t="s" s="2">
         <v>41</v>
       </c>
@@ -3036,13 +3228,13 @@
         <v>41</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>41</v>
+        <v>150</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>41</v>
+        <v>151</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>41</v>
+        <v>152</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>41</v>
@@ -3060,7 +3252,7 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>39</v>
@@ -3075,15 +3267,15 @@
         <v>41</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3091,13 +3283,13 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>41</v>
@@ -3106,24 +3298,26 @@
         <v>48</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>66</v>
+        <v>156</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>166</v>
-      </c>
-      <c r="M22" s="2"/>
+        <v>158</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>159</v>
+      </c>
       <c r="N22" t="s" s="2">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
-        <v>168</v>
+        <v>41</v>
       </c>
       <c r="R22" t="s" s="2">
         <v>41</v>
@@ -3141,13 +3335,13 @@
         <v>41</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>41</v>
+        <v>161</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>41</v>
+        <v>162</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>41</v>
+        <v>163</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>41</v>
@@ -3165,7 +3359,7 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
@@ -3180,7 +3374,7 @@
         <v>41</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>128</v>
+        <v>154</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>41</v>
@@ -3188,7 +3382,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3211,17 +3405,19 @@
         <v>48</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>131</v>
+        <v>60</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>172</v>
-      </c>
-      <c r="M23" s="2"/>
+        <v>167</v>
+      </c>
+      <c r="M23" t="s" s="2">
+        <v>168</v>
+      </c>
       <c r="N23" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -3234,7 +3430,7 @@
         <v>41</v>
       </c>
       <c r="S23" t="s" s="2">
-        <v>41</v>
+        <v>170</v>
       </c>
       <c r="T23" t="s" s="2">
         <v>41</v>
@@ -3270,7 +3466,7 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
@@ -3285,7 +3481,7 @@
         <v>41</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>41</v>
@@ -3293,7 +3489,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3316,20 +3512,18 @@
         <v>48</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>177</v>
+        <v>120</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>180</v>
-      </c>
-      <c r="N24" t="s" s="2">
-        <v>181</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="N24" s="2"/>
       <c r="O24" t="s" s="2">
         <v>41</v>
       </c>
@@ -3341,7 +3535,7 @@
         <v>41</v>
       </c>
       <c r="S24" t="s" s="2">
-        <v>41</v>
+        <v>177</v>
       </c>
       <c r="T24" t="s" s="2">
         <v>41</v>
@@ -3377,7 +3571,7 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3392,7 +3586,7 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>41</v>
@@ -3400,7 +3594,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3423,20 +3617,16 @@
         <v>48</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>131</v>
+        <v>181</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>186</v>
-      </c>
-      <c r="M25" t="s" s="2">
-        <v>187</v>
-      </c>
-      <c r="N25" t="s" s="2">
-        <v>188</v>
-      </c>
+        <v>183</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
       <c r="O25" t="s" s="2">
         <v>41</v>
       </c>
@@ -3484,7 +3674,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3499,15 +3689,15 @@
         <v>41</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3515,13 +3705,13 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>41</v>
@@ -3530,20 +3720,18 @@
         <v>48</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>195</v>
-      </c>
-      <c r="N26" t="s" s="2">
-        <v>196</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="N26" s="2"/>
       <c r="O26" t="s" s="2">
         <v>41</v>
       </c>
@@ -3606,15 +3794,15 @@
         <v>41</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>198</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3622,7 +3810,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>47</v>
@@ -3631,23 +3819,25 @@
         <v>41</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>200</v>
+        <v>156</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="M27" s="2"/>
+        <v>195</v>
+      </c>
+      <c r="M27" t="s" s="2">
+        <v>196</v>
+      </c>
       <c r="N27" t="s" s="2">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>41</v>
@@ -3672,13 +3862,13 @@
         <v>41</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>41</v>
+        <v>198</v>
       </c>
       <c r="X27" t="s" s="2">
-        <v>41</v>
+        <v>199</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>41</v>
+        <v>200</v>
       </c>
       <c r="Z27" t="s" s="2">
         <v>41</v>
@@ -3696,10 +3886,10 @@
         <v>41</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>47</v>
@@ -3711,15 +3901,15 @@
         <v>41</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3739,21 +3929,19 @@
         <v>41</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>207</v>
+        <v>120</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>208</v>
+        <v>121</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>209</v>
+        <v>122</v>
       </c>
       <c r="M28" s="2"/>
-      <c r="N28" t="s" s="2">
-        <v>210</v>
-      </c>
+      <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
         <v>41</v>
       </c>
@@ -3801,29 +3989,1402 @@
         <v>41</v>
       </c>
       <c r="AE28" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="AF28" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG28" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI28" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ28" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AK28" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="29" hidden="true">
+      <c r="A29" t="s" s="2">
+        <v>204</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="D29" s="2"/>
+      <c r="E29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J29" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K29" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="L29" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M29" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="N29" s="2"/>
+      <c r="O29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P29" s="2"/>
+      <c r="Q29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA29" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AB29" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="AC29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD29" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AE29" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AF29" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG29" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI29" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ29" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AK29" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s" s="2">
+        <v>205</v>
+      </c>
+      <c r="B30" s="2"/>
+      <c r="C30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D30" s="2"/>
+      <c r="E30" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G30" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="H30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I30" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J30" t="s" s="2">
         <v>206</v>
       </c>
-      <c r="AF28" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG28" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI28" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ28" t="s" s="2">
+      <c r="K30" t="s" s="2">
+        <v>207</v>
+      </c>
+      <c r="L30" t="s" s="2">
+        <v>208</v>
+      </c>
+      <c r="M30" t="s" s="2">
+        <v>209</v>
+      </c>
+      <c r="N30" t="s" s="2">
+        <v>210</v>
+      </c>
+      <c r="O30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P30" s="2"/>
+      <c r="Q30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE30" t="s" s="2">
         <v>211</v>
       </c>
-      <c r="AK28" t="s" s="2">
+      <c r="AF30" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG30" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI30" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ30" t="s" s="2">
         <v>212</v>
+      </c>
+      <c r="AK30" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" hidden="true">
+      <c r="A31" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="B31" s="2"/>
+      <c r="C31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D31" s="2"/>
+      <c r="E31" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F31" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J31" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="K31" t="s" s="2">
+        <v>121</v>
+      </c>
+      <c r="L31" t="s" s="2">
+        <v>122</v>
+      </c>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2"/>
+      <c r="O31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P31" s="2"/>
+      <c r="Q31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE31" t="s" s="2">
+        <v>123</v>
+      </c>
+      <c r="AF31" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG31" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI31" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ31" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AK31" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" hidden="true">
+      <c r="A32" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="B32" s="2"/>
+      <c r="C32" t="s" s="2">
+        <v>108</v>
+      </c>
+      <c r="D32" s="2"/>
+      <c r="E32" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="G32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="J32" t="s" s="2">
+        <v>91</v>
+      </c>
+      <c r="K32" t="s" s="2">
+        <v>126</v>
+      </c>
+      <c r="L32" t="s" s="2">
+        <v>127</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>111</v>
+      </c>
+      <c r="N32" s="2"/>
+      <c r="O32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P32" s="2"/>
+      <c r="Q32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA32" t="s" s="2">
+        <v>94</v>
+      </c>
+      <c r="AB32" t="s" s="2">
+        <v>128</v>
+      </c>
+      <c r="AC32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD32" t="s" s="2">
+        <v>95</v>
+      </c>
+      <c r="AE32" t="s" s="2">
+        <v>129</v>
+      </c>
+      <c r="AF32" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG32" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="AH32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI32" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ32" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="AK32" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" hidden="true">
+      <c r="A33" t="s" s="2">
+        <v>215</v>
+      </c>
+      <c r="B33" s="2"/>
+      <c r="C33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D33" s="2"/>
+      <c r="E33" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F33" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I33" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J33" t="s" s="2">
+        <v>60</v>
+      </c>
+      <c r="K33" t="s" s="2">
+        <v>216</v>
+      </c>
+      <c r="L33" t="s" s="2">
+        <v>217</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>218</v>
+      </c>
+      <c r="N33" t="s" s="2">
+        <v>219</v>
+      </c>
+      <c r="O33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P33" s="2"/>
+      <c r="Q33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE33" t="s" s="2">
+        <v>220</v>
+      </c>
+      <c r="AF33" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG33" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI33" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ33" t="s" s="2">
+        <v>221</v>
+      </c>
+      <c r="AK33" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="34" hidden="true">
+      <c r="A34" t="s" s="2">
+        <v>222</v>
+      </c>
+      <c r="B34" s="2"/>
+      <c r="C34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D34" s="2"/>
+      <c r="E34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F34" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I34" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J34" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="K34" t="s" s="2">
+        <v>223</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>224</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>225</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P34" s="2"/>
+      <c r="Q34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE34" t="s" s="2">
+        <v>226</v>
+      </c>
+      <c r="AF34" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG34" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI34" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ34" t="s" s="2">
+        <v>227</v>
+      </c>
+      <c r="AK34" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s" s="2">
+        <v>228</v>
+      </c>
+      <c r="B35" s="2"/>
+      <c r="C35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D35" s="2"/>
+      <c r="E35" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="F35" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G35" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="H35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I35" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J35" t="s" s="2">
+        <v>66</v>
+      </c>
+      <c r="K35" t="s" s="2">
+        <v>229</v>
+      </c>
+      <c r="L35" t="s" s="2">
+        <v>230</v>
+      </c>
+      <c r="M35" s="2"/>
+      <c r="N35" t="s" s="2">
+        <v>231</v>
+      </c>
+      <c r="O35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P35" s="2"/>
+      <c r="Q35" t="s" s="2">
+        <v>232</v>
+      </c>
+      <c r="R35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE35" t="s" s="2">
+        <v>233</v>
+      </c>
+      <c r="AF35" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG35" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI35" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ35" t="s" s="2">
+        <v>201</v>
+      </c>
+      <c r="AK35" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" hidden="true">
+      <c r="A36" t="s" s="2">
+        <v>234</v>
+      </c>
+      <c r="B36" s="2"/>
+      <c r="C36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D36" s="2"/>
+      <c r="E36" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F36" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I36" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J36" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="K36" t="s" s="2">
+        <v>235</v>
+      </c>
+      <c r="L36" t="s" s="2">
+        <v>236</v>
+      </c>
+      <c r="M36" s="2"/>
+      <c r="N36" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="O36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P36" s="2"/>
+      <c r="Q36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE36" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="AF36" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG36" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI36" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ36" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="AK36" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" hidden="true">
+      <c r="A37" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F37" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I37" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J37" t="s" s="2">
+        <v>241</v>
+      </c>
+      <c r="K37" t="s" s="2">
+        <v>242</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>243</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>244</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>245</v>
+      </c>
+      <c r="O37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P37" s="2"/>
+      <c r="Q37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE37" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="AF37" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG37" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI37" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ37" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="AK37" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="38" hidden="true">
+      <c r="A38" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F38" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I38" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J38" t="s" s="2">
+        <v>120</v>
+      </c>
+      <c r="K38" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>250</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>251</v>
+      </c>
+      <c r="N38" t="s" s="2">
+        <v>252</v>
+      </c>
+      <c r="O38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P38" s="2"/>
+      <c r="Q38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE38" t="s" s="2">
+        <v>253</v>
+      </c>
+      <c r="AF38" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG38" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI38" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ38" t="s" s="2">
+        <v>254</v>
+      </c>
+      <c r="AK38" t="s" s="2">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="B39" s="2"/>
+      <c r="C39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D39" s="2"/>
+      <c r="E39" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="F39" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G39" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="H39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I39" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J39" t="s" s="2">
+        <v>256</v>
+      </c>
+      <c r="K39" t="s" s="2">
+        <v>257</v>
+      </c>
+      <c r="L39" t="s" s="2">
+        <v>258</v>
+      </c>
+      <c r="M39" t="s" s="2">
+        <v>259</v>
+      </c>
+      <c r="N39" t="s" s="2">
+        <v>260</v>
+      </c>
+      <c r="O39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P39" s="2"/>
+      <c r="Q39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE39" t="s" s="2">
+        <v>255</v>
+      </c>
+      <c r="AF39" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG39" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI39" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ39" t="s" s="2">
+        <v>261</v>
+      </c>
+      <c r="AK39" t="s" s="2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="40" hidden="true">
+      <c r="A40" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="B40" s="2"/>
+      <c r="C40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D40" s="2"/>
+      <c r="E40" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F40" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I40" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J40" t="s" s="2">
+        <v>264</v>
+      </c>
+      <c r="K40" t="s" s="2">
+        <v>265</v>
+      </c>
+      <c r="L40" t="s" s="2">
+        <v>266</v>
+      </c>
+      <c r="M40" s="2"/>
+      <c r="N40" t="s" s="2">
+        <v>267</v>
+      </c>
+      <c r="O40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P40" s="2"/>
+      <c r="Q40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE40" t="s" s="2">
+        <v>263</v>
+      </c>
+      <c r="AF40" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG40" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI40" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ40" t="s" s="2">
+        <v>268</v>
+      </c>
+      <c r="AK40" t="s" s="2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" hidden="true">
+      <c r="A41" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="B41" s="2"/>
+      <c r="C41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="D41" s="2"/>
+      <c r="E41" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="F41" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="G41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="H41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="I41" t="s" s="2">
+        <v>48</v>
+      </c>
+      <c r="J41" t="s" s="2">
+        <v>271</v>
+      </c>
+      <c r="K41" t="s" s="2">
+        <v>272</v>
+      </c>
+      <c r="L41" t="s" s="2">
+        <v>273</v>
+      </c>
+      <c r="M41" s="2"/>
+      <c r="N41" t="s" s="2">
+        <v>274</v>
+      </c>
+      <c r="O41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="P41" s="2"/>
+      <c r="Q41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="R41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="S41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="T41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="U41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="V41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="W41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="X41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE41" t="s" s="2">
+        <v>270</v>
+      </c>
+      <c r="AF41" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="AG41" t="s" s="2">
+        <v>47</v>
+      </c>
+      <c r="AH41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AI41" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AJ41" t="s" s="2">
+        <v>275</v>
+      </c>
+      <c r="AK41" t="s" s="2">
+        <v>276</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK28">
+  <autoFilter ref="A1:AK41">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -3833,7 +5394,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI27">
+  <conditionalFormatting sqref="A2:AI40">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>

<commit_message>
update capstatements to R4
</commit_message>
<xml_diff>
--- a/docs/template-basic.xlsx
+++ b/docs/template-basic.xlsx
@@ -371,7 +371,7 @@
     <t>There can be no stigma associated with the use of extensions by any application, project, or standard - regardless of the institution or jurisdiction that uses or defines the extensions.  The use of extensions is what allows the FHIR specification to retain a core level of simplicity for everyone.</t>
   </si>
   <si>
-    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](extensibility.html#modifierExtension).</t>
+    <t>Modifier extensions allow for extensions that *cannot* be safely ignored to be clearly distinguished from the vast majority of extensions which can be safely ignored.  This promotes interoperability by eliminating the need for implementers to prohibit the presence of extensions. For further information, see the [definition of modifier extensions](http://build.fhir.org/extensibility.html#modifierExtension).</t>
   </si>
   <si>
     <t>DomainResource.modifierExtension</t>
@@ -472,7 +472,7 @@
     <t>Value of extension</t>
   </si>
   <si>
-    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](extensibility.html) for a list).</t>
+    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://build.fhir.org/extensibility.html) for a list).</t>
   </si>
   <si>
     <t>Extension.value[x]</t>
@@ -572,7 +572,7 @@
     <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
   </si>
   <si>
-    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
+    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](http://build.fhir.org/extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
   </si>
   <si>
     <t>&lt;valueString xmlns="http://hl7.org/fhir" value="123456"/&gt;</t>

</xml_diff>

<commit_message>
add example fix template
</commit_message>
<xml_diff>
--- a/docs/template-basic.xlsx
+++ b/docs/template-basic.xlsx
@@ -9,13 +9,13 @@
     <sheet name="Elements" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">Elements!$A$1:$AK$28</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="214">
   <si>
     <t>Path</t>
   </si>
@@ -396,7 +396,42 @@
     <t>FiveWs.identifier</t>
   </si>
   <si>
-    <t>Basic.identifier.id</t>
+    <t>Basic.code</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CodeableConcept {[]} {[]}
+</t>
+  </si>
+  <si>
+    <t>Kind of Resource</t>
+  </si>
+  <si>
+    <t>Identifies the 'type' of resource - equivalent to the resource name for other resources.</t>
+  </si>
+  <si>
+    <t>Because resource references will only be able to indicate 'Basic', the type of reference will need to be specified in a Profile identified as part of the resource.  Refer to the resource notes section for information on appropriate terminologies for this code.
+This element is labeled as a modifier because it defines the meaning of the resource and cannot be ignored.</t>
+  </si>
+  <si>
+    <t>Must be able to distinguish different types of Basic resources.</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>Codes for identifying types of resources not yet defined by FHIR.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/ValueSet/basic-resource-type</t>
+  </si>
+  <si>
+    <t>./code</t>
+  </si>
+  <si>
+    <t>FiveWs.what[x]</t>
+  </si>
+  <si>
+    <t>Basic.code.id</t>
   </si>
   <si>
     <t xml:space="preserve">string {[]} {[]}
@@ -415,7 +450,7 @@
     <t>n/a</t>
   </si>
   <si>
-    <t>Basic.identifier.extension</t>
+    <t>Basic.code.extension</t>
   </si>
   <si>
     <t>Additional content defined by implementations</t>
@@ -428,238 +463,6 @@
   </si>
   <si>
     <t>Element.extension</t>
-  </si>
-  <si>
-    <t>foo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Extension {[CanonicalType[http://www.fhir.org/guides/test3/StructureDefinition/extension-identifier-status]]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Basic.identifier.extension.id</t>
-  </si>
-  <si>
-    <t>Basic.identifier.extension.extension</t>
-  </si>
-  <si>
-    <t>Basic.identifier.extension.url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">null {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>identifies the meaning of the extension</t>
-  </si>
-  <si>
-    <t>Source of the definition for the extension code - a logical name or a URL.</t>
-  </si>
-  <si>
-    <t>The definition may point directly to a computable or human-readable definition of the extensibility codes, or it may be a logical URI as declared in some other specification. The definition SHALL be a URI for the Structure Definition defining the extension.</t>
-  </si>
-  <si>
-    <t>Extension.url</t>
-  </si>
-  <si>
-    <t>Basic.identifier.extension.value[x]</t>
-  </si>
-  <si>
-    <t>base64Binary {[]} {[]}
-boolean {[]} {[]}canonical {[]} {[]}code {[]} {[]}date {[]} {[]}dateTime {[]} {[]}decimal {[]} {[]}id {[]} {[]}instant {[]} {[]}integer {[]} {[]}markdown {[]} {[]}oid {[]} {[]}positiveInt {[]} {[]}string {[]} {[]}time {[]} {[]}unsignedInt {[]} {[]}uri {[]} {[]}url {[]} {[]}uuid {[]} {[]}Address {[]} {[]}Age {[]} {[]}Annotation {[]} {[]}Attachment {[]} {[]}CodeableConcept {[]} {[]}Coding {[]} {[]}ContactPoint {[]} {[]}Count {[]} {[]}Distance {[]} {[]}Duration {[]} {[]}HumanName {[]} {[]}Identifier {[]} {[]}Money {[]} {[]}Period {[]} {[]}Quantity {[]} {[]}Range {[]} {[]}Ratio {[]} {[]}Reference {[]} {[]}SampledData {[]} {[]}Signature {[]} {[]}Timing {[]} {[]}ContactDetail {[]} {[]}Contributor {[]} {[]}DataRequirement {[]} {[]}Expression {[]} {[]}ParameterDefinition {[]} {[]}RelatedArtifact {[]} {[]}TriggerDefinition {[]} {[]}UsageContext {[]} {[]}Dosage {[]} {[]}</t>
-  </si>
-  <si>
-    <t>Value of extension</t>
-  </si>
-  <si>
-    <t>Value of extension - must be one of a constrained set of the data types (see [Extensibility](http://build.fhir.org/extensibility.html) for a list).</t>
-  </si>
-  <si>
-    <t>Extension.value[x]</t>
-  </si>
-  <si>
-    <t>Basic.identifier.use</t>
-  </si>
-  <si>
-    <t>usual | official | temp | secondary | old (If known)</t>
-  </si>
-  <si>
-    <t>The purpose of this identifier.</t>
-  </si>
-  <si>
-    <t>Applications can assume that an identifier is permanent unless it explicitly says that it is temporary.</t>
-  </si>
-  <si>
-    <t>Allows the appropriate identifier for a particular context of use to be selected from among a set of identifiers.</t>
-  </si>
-  <si>
-    <t>required</t>
-  </si>
-  <si>
-    <t>Identifies the purpose for this identifier, if known .</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-use|4.0.0</t>
-  </si>
-  <si>
-    <t>Identifier.use</t>
-  </si>
-  <si>
-    <t>Role.code or implied by context</t>
-  </si>
-  <si>
-    <t>Basic.identifier.type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CodeableConcept {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Description of identifier</t>
-  </si>
-  <si>
-    <t>A coded type for the identifier that can be used to determine which identifier to use for a specific purpose.</t>
-  </si>
-  <si>
-    <t>This element deals only with general categories of identifiers.  It SHOULD not be used for codes that correspond 1..1 with the Identifier.system. Some identifiers may fall into multiple categories due to common usage.   Where the system is known, a type is unnecessary because the type is always part of the system definition. However systems often need to handle identifiers where the system is not known. There is not a 1:1 relationship between type and system, since many different systems have the same type.</t>
-  </si>
-  <si>
-    <t>Allows users to make use of identifiers when the identifier system is not known.</t>
-  </si>
-  <si>
-    <t>extensible</t>
-  </si>
-  <si>
-    <t>A coded type for an identifier that can be used to determine which identifier to use for a specific purpose.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/identifier-type</t>
-  </si>
-  <si>
-    <t>Identifier.type</t>
-  </si>
-  <si>
-    <t>Basic.identifier.system</t>
-  </si>
-  <si>
-    <t>The namespace for the identifier value</t>
-  </si>
-  <si>
-    <t>Establishes the namespace for the value - that is, a URL that describes a set values that are unique.</t>
-  </si>
-  <si>
-    <t>Identifier.system is always case sensitive.</t>
-  </si>
-  <si>
-    <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
-  </si>
-  <si>
-    <t>&lt;valueUri xmlns="http://hl7.org/fhir" value="http://www.acme.com/identifiers/patient"/&gt;</t>
-  </si>
-  <si>
-    <t>Identifier.system</t>
-  </si>
-  <si>
-    <t>II.root or Role.id.root</t>
-  </si>
-  <si>
-    <t>Basic.identifier.value</t>
-  </si>
-  <si>
-    <t>The value that is unique</t>
-  </si>
-  <si>
-    <t>The portion of the identifier typically relevant to the user and which is unique within the context of the system.</t>
-  </si>
-  <si>
-    <t>If the value is a full URI, then the system SHALL be urn:ietf:rfc:3986.  The value's primary purpose is computational mapping.  As a result, it may be normalized for comparison purposes (e.g. removing non-significant whitespace, dashes, etc.)  A value formatted for human display can be conveyed using the [Rendered Value extension](http://build.fhir.org/extension-rendered-value.html). Identifier.value is to be treated as case sensitive unless knowledge of the Identifier.system allows the processer to be confident that non-case-sensitive processing is safe.</t>
-  </si>
-  <si>
-    <t>&lt;valueString xmlns="http://hl7.org/fhir" value="123456"/&gt;</t>
-  </si>
-  <si>
-    <t>Identifier.value</t>
-  </si>
-  <si>
-    <t>II.extension or II.root if system indicates OID or GUID (Or Role.id.extension or root)</t>
-  </si>
-  <si>
-    <t>Basic.identifier.period</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Period {[]} {[]}
-</t>
-  </si>
-  <si>
-    <t>Time period when id is/was valid for use</t>
-  </si>
-  <si>
-    <t>Time period during which identifier is/was valid for use.</t>
-  </si>
-  <si>
-    <t>Identifier.period</t>
-  </si>
-  <si>
-    <t>Role.effectiveTime or implied by context</t>
-  </si>
-  <si>
-    <t>Basic.identifier.assigner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reference {[]} {[CanonicalType[http://hl7.org/fhir/StructureDefinition/Organization]]}
-</t>
-  </si>
-  <si>
-    <t>Organization that issued id (may be just text)</t>
-  </si>
-  <si>
-    <t>Organization that issued/manages the identifier.</t>
-  </si>
-  <si>
-    <t>The Identifier.assigner may omit the .reference element and only contain a .display element reflecting the name or other textual information about the assigning organization.</t>
-  </si>
-  <si>
-    <t>Identifier.assigner</t>
-  </si>
-  <si>
-    <t>II.assigningAuthorityName but note that this is an improper use by the definition of the field.  Also Role.scoper</t>
-  </si>
-  <si>
-    <t>Basic.code</t>
-  </si>
-  <si>
-    <t>Kind of Resource</t>
-  </si>
-  <si>
-    <t>Identifies the 'type' of resource - equivalent to the resource name for other resources.</t>
-  </si>
-  <si>
-    <t>Because resource references will only be able to indicate 'Basic', the type of reference will need to be specified in a Profile identified as part of the resource.  Refer to the resource notes section for information on appropriate terminologies for this code.
-This element is labeled as a modifier because it defines the meaning of the resource and cannot be ignored.</t>
-  </si>
-  <si>
-    <t>Must be able to distinguish different types of Basic resources.</t>
-  </si>
-  <si>
-    <t>example</t>
-  </si>
-  <si>
-    <t>Codes for identifying types of resources not yet defined by FHIR.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/basic-resource-type</t>
-  </si>
-  <si>
-    <t>./code</t>
-  </si>
-  <si>
-    <t>FiveWs.what[x]</t>
-  </si>
-  <si>
-    <t>Basic.code.id</t>
-  </si>
-  <si>
-    <t>Basic.code.extension</t>
   </si>
   <si>
     <t>Basic.code.coding</t>
@@ -1029,7 +832,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AK41"/>
+  <dimension ref="A1:AK28"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane xSplit="2.0" ySplit="1.0" state="frozen" topLeftCell="C2" activePane="bottomRight"/>
@@ -1038,7 +841,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="32.7265625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="28.7265625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="18.5859375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="38.45703125" customWidth="true" bestFit="true" hidden="true"/>
     <col min="4" max="4" width="6.14453125" customWidth="true" bestFit="true" hidden="true"/>
@@ -1061,7 +864,7 @@
     <col min="21" max="21" width="16.1328125" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.40234375" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="16.95703125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="95.39453125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="58.5859375" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="45.39453125" customWidth="true" bestFit="true"/>
     <col min="26" max="26" width="5.8828125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="20.83984375" customWidth="true" bestFit="true"/>
@@ -1073,7 +876,7 @@
     <col min="33" max="33" width="9.890625" customWidth="true" bestFit="true" hidden="true"/>
     <col min="34" max="34" width="12.71875" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="36" max="36" width="99.8984375" customWidth="true" bestFit="true"/>
+    <col min="36" max="36" width="71.09375" customWidth="true" bestFit="true"/>
     <col min="37" max="37" width="33.046875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -2452,7 +2255,7 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F14" t="s" s="2">
         <v>47</v>
@@ -2461,10 +2264,10 @@
         <v>41</v>
       </c>
       <c r="H14" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="I14" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J14" t="s" s="2">
         <v>121</v>
@@ -2475,8 +2278,12 @@
       <c r="L14" t="s" s="2">
         <v>123</v>
       </c>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="M14" t="s" s="2">
+        <v>124</v>
+      </c>
+      <c r="N14" t="s" s="2">
+        <v>125</v>
+      </c>
       <c r="O14" t="s" s="2">
         <v>41</v>
       </c>
@@ -2500,13 +2307,13 @@
         <v>41</v>
       </c>
       <c r="W14" t="s" s="2">
-        <v>41</v>
+        <v>126</v>
       </c>
       <c r="X14" t="s" s="2">
-        <v>41</v>
+        <v>127</v>
       </c>
       <c r="Y14" t="s" s="2">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="Z14" t="s" s="2">
         <v>41</v>
@@ -2524,10 +2331,10 @@
         <v>41</v>
       </c>
       <c r="AE14" t="s" s="2">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>47</v>
@@ -2539,26 +2346,26 @@
         <v>41</v>
       </c>
       <c r="AJ14" t="s" s="2">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>41</v>
+        <v>130</v>
       </c>
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" t="s" s="2">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F15" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G15" t="s" s="2">
         <v>41</v>
@@ -2570,17 +2377,15 @@
         <v>41</v>
       </c>
       <c r="J15" t="s" s="2">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="K15" t="s" s="2">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="M15" t="s" s="2">
-        <v>111</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="M15" s="2"/>
       <c r="N15" s="2"/>
       <c r="O15" t="s" s="2">
         <v>41</v>
@@ -2617,25 +2422,25 @@
         <v>41</v>
       </c>
       <c r="AA15" t="s" s="2">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="AB15" t="s" s="2">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="AC15" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD15" t="s" s="2">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="AE15" t="s" s="2">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="AF15" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG15" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH15" t="s" s="2">
         <v>41</v>
@@ -2644,31 +2449,29 @@
         <v>41</v>
       </c>
       <c r="AJ15" t="s" s="2">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="AK15" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>126</v>
-      </c>
-      <c r="B16" t="s" s="2">
-        <v>131</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="B16" s="2"/>
       <c r="C16" t="s" s="2">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F16" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="H16" t="s" s="2">
         <v>41</v>
@@ -2677,15 +2480,17 @@
         <v>41</v>
       </c>
       <c r="J16" t="s" s="2">
-        <v>132</v>
+        <v>91</v>
       </c>
       <c r="K16" t="s" s="2">
-        <v>92</v>
+        <v>138</v>
       </c>
       <c r="L16" t="s" s="2">
-        <v>93</v>
-      </c>
-      <c r="M16" s="2"/>
+        <v>139</v>
+      </c>
+      <c r="M16" t="s" s="2">
+        <v>111</v>
+      </c>
       <c r="N16" s="2"/>
       <c r="O16" t="s" s="2">
         <v>41</v>
@@ -2722,19 +2527,19 @@
         <v>41</v>
       </c>
       <c r="AA16" t="s" s="2">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="AB16" t="s" s="2">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="AC16" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD16" t="s" s="2">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="AE16" t="s" s="2">
-        <v>130</v>
+        <v>141</v>
       </c>
       <c r="AF16" t="s" s="2">
         <v>39</v>
@@ -2749,15 +2554,15 @@
         <v>41</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>41</v>
+        <v>136</v>
       </c>
       <c r="AK16" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="17" hidden="true">
+    <row r="17">
       <c r="A17" t="s" s="2">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" t="s" s="2">
@@ -2765,31 +2570,35 @@
       </c>
       <c r="D17" s="2"/>
       <c r="E17" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F17" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G17" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H17" t="s" s="2">
         <v>41</v>
       </c>
       <c r="I17" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J17" t="s" s="2">
-        <v>121</v>
+        <v>143</v>
       </c>
       <c r="K17" t="s" s="2">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
+        <v>145</v>
+      </c>
+      <c r="M17" t="s" s="2">
+        <v>146</v>
+      </c>
+      <c r="N17" t="s" s="2">
+        <v>147</v>
+      </c>
       <c r="O17" t="s" s="2">
         <v>41</v>
       </c>
@@ -2837,13 +2646,13 @@
         <v>41</v>
       </c>
       <c r="AE17" t="s" s="2">
-        <v>124</v>
+        <v>148</v>
       </c>
       <c r="AF17" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG17" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH17" t="s" s="2">
         <v>41</v>
@@ -2852,7 +2661,7 @@
         <v>41</v>
       </c>
       <c r="AJ17" t="s" s="2">
-        <v>125</v>
+        <v>149</v>
       </c>
       <c r="AK17" t="s" s="2">
         <v>41</v>
@@ -2860,18 +2669,18 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" t="s" s="2">
-        <v>108</v>
+        <v>41</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="F18" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="G18" t="s" s="2">
         <v>41</v>
@@ -2883,17 +2692,15 @@
         <v>41</v>
       </c>
       <c r="J18" t="s" s="2">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="M18" t="s" s="2">
-        <v>111</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="M18" s="2"/>
       <c r="N18" s="2"/>
       <c r="O18" t="s" s="2">
         <v>41</v>
@@ -2930,25 +2737,25 @@
         <v>41</v>
       </c>
       <c r="AA18" t="s" s="2">
-        <v>94</v>
+        <v>41</v>
       </c>
       <c r="AB18" t="s" s="2">
-        <v>129</v>
+        <v>41</v>
       </c>
       <c r="AC18" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD18" t="s" s="2">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="AE18" t="s" s="2">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="AF18" t="s" s="2">
         <v>39</v>
       </c>
       <c r="AG18" t="s" s="2">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AH18" t="s" s="2">
         <v>41</v>
@@ -2957,7 +2764,7 @@
         <v>41</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="AK18" t="s" s="2">
         <v>41</v>
@@ -2965,18 +2772,18 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>135</v>
+        <v>151</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" t="s" s="2">
-        <v>41</v>
+        <v>108</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F19" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="G19" t="s" s="2">
         <v>41</v>
@@ -2988,16 +2795,16 @@
         <v>41</v>
       </c>
       <c r="J19" t="s" s="2">
-        <v>136</v>
+        <v>91</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" t="s" s="2">
@@ -3035,25 +2842,25 @@
         <v>41</v>
       </c>
       <c r="AA19" t="s" s="2">
-        <v>41</v>
+        <v>94</v>
       </c>
       <c r="AB19" t="s" s="2">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="AC19" t="s" s="2">
         <v>41</v>
       </c>
       <c r="AD19" t="s" s="2">
-        <v>41</v>
+        <v>95</v>
       </c>
       <c r="AE19" t="s" s="2">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG19" t="s" s="2">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="AH19" t="s" s="2">
         <v>41</v>
@@ -3062,7 +2869,7 @@
         <v>41</v>
       </c>
       <c r="AJ19" t="s" s="2">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="AK19" t="s" s="2">
         <v>41</v>
@@ -3070,7 +2877,7 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>141</v>
+        <v>152</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" t="s" s="2">
@@ -3090,19 +2897,23 @@
         <v>41</v>
       </c>
       <c r="I20" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J20" t="s" s="2">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>144</v>
-      </c>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+        <v>154</v>
+      </c>
+      <c r="M20" t="s" s="2">
+        <v>155</v>
+      </c>
+      <c r="N20" t="s" s="2">
+        <v>156</v>
+      </c>
       <c r="O20" t="s" s="2">
         <v>41</v>
       </c>
@@ -3150,7 +2961,7 @@
         <v>41</v>
       </c>
       <c r="AE20" t="s" s="2">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="AF20" t="s" s="2">
         <v>39</v>
@@ -3165,7 +2976,7 @@
         <v>41</v>
       </c>
       <c r="AJ20" t="s" s="2">
-        <v>89</v>
+        <v>158</v>
       </c>
       <c r="AK20" t="s" s="2">
         <v>41</v>
@@ -3173,7 +2984,7 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" t="s" s="2">
@@ -3190,26 +3001,24 @@
         <v>41</v>
       </c>
       <c r="H21" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I21" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J21" t="s" s="2">
-        <v>66</v>
+        <v>132</v>
       </c>
       <c r="K21" t="s" s="2">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="L21" t="s" s="2">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="M21" t="s" s="2">
-        <v>149</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>150</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="N21" s="2"/>
       <c r="O21" t="s" s="2">
         <v>41</v>
       </c>
@@ -3233,13 +3042,13 @@
         <v>41</v>
       </c>
       <c r="W21" t="s" s="2">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="X21" t="s" s="2">
-        <v>152</v>
+        <v>41</v>
       </c>
       <c r="Y21" t="s" s="2">
-        <v>153</v>
+        <v>41</v>
       </c>
       <c r="Z21" t="s" s="2">
         <v>41</v>
@@ -3257,7 +3066,7 @@
         <v>41</v>
       </c>
       <c r="AE21" t="s" s="2">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="AF21" t="s" s="2">
         <v>39</v>
@@ -3272,15 +3081,15 @@
         <v>41</v>
       </c>
       <c r="AJ21" t="s" s="2">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="AK21" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="22" hidden="true">
+    <row r="22">
       <c r="A22" t="s" s="2">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" t="s" s="2">
@@ -3288,13 +3097,13 @@
       </c>
       <c r="D22" s="2"/>
       <c r="E22" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F22" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G22" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H22" t="s" s="2">
         <v>41</v>
@@ -3303,26 +3112,24 @@
         <v>48</v>
       </c>
       <c r="J22" t="s" s="2">
-        <v>157</v>
+        <v>66</v>
       </c>
       <c r="K22" t="s" s="2">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="L22" t="s" s="2">
-        <v>159</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>160</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="M22" s="2"/>
       <c r="N22" t="s" s="2">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="O22" t="s" s="2">
         <v>41</v>
       </c>
       <c r="P22" s="2"/>
       <c r="Q22" t="s" s="2">
-        <v>41</v>
+        <v>169</v>
       </c>
       <c r="R22" t="s" s="2">
         <v>41</v>
@@ -3340,13 +3147,13 @@
         <v>41</v>
       </c>
       <c r="W22" t="s" s="2">
-        <v>162</v>
+        <v>41</v>
       </c>
       <c r="X22" t="s" s="2">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="Y22" t="s" s="2">
-        <v>164</v>
+        <v>41</v>
       </c>
       <c r="Z22" t="s" s="2">
         <v>41</v>
@@ -3364,7 +3171,7 @@
         <v>41</v>
       </c>
       <c r="AE22" t="s" s="2">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="AF22" t="s" s="2">
         <v>39</v>
@@ -3379,7 +3186,7 @@
         <v>41</v>
       </c>
       <c r="AJ22" t="s" s="2">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="AK22" t="s" s="2">
         <v>41</v>
@@ -3387,7 +3194,7 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" t="s" s="2">
@@ -3410,19 +3217,17 @@
         <v>48</v>
       </c>
       <c r="J23" t="s" s="2">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>168</v>
-      </c>
-      <c r="M23" t="s" s="2">
-        <v>169</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="M23" s="2"/>
       <c r="N23" t="s" s="2">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="O23" t="s" s="2">
         <v>41</v>
@@ -3435,7 +3240,7 @@
         <v>41</v>
       </c>
       <c r="S23" t="s" s="2">
-        <v>171</v>
+        <v>41</v>
       </c>
       <c r="T23" t="s" s="2">
         <v>41</v>
@@ -3471,7 +3276,7 @@
         <v>41</v>
       </c>
       <c r="AE23" t="s" s="2">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="AF23" t="s" s="2">
         <v>39</v>
@@ -3486,7 +3291,7 @@
         <v>41</v>
       </c>
       <c r="AJ23" t="s" s="2">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AK23" t="s" s="2">
         <v>41</v>
@@ -3494,7 +3299,7 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" t="s" s="2">
@@ -3517,18 +3322,20 @@
         <v>48</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>177</v>
-      </c>
-      <c r="N24" s="2"/>
+        <v>181</v>
+      </c>
+      <c r="N24" t="s" s="2">
+        <v>182</v>
+      </c>
       <c r="O24" t="s" s="2">
         <v>41</v>
       </c>
@@ -3540,7 +3347,7 @@
         <v>41</v>
       </c>
       <c r="S24" t="s" s="2">
-        <v>178</v>
+        <v>41</v>
       </c>
       <c r="T24" t="s" s="2">
         <v>41</v>
@@ -3576,7 +3383,7 @@
         <v>41</v>
       </c>
       <c r="AE24" t="s" s="2">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="AF24" t="s" s="2">
         <v>39</v>
@@ -3591,7 +3398,7 @@
         <v>41</v>
       </c>
       <c r="AJ24" t="s" s="2">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="AK24" t="s" s="2">
         <v>41</v>
@@ -3599,7 +3406,7 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -3622,16 +3429,20 @@
         <v>48</v>
       </c>
       <c r="J25" t="s" s="2">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>184</v>
-      </c>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+        <v>187</v>
+      </c>
+      <c r="M25" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="N25" t="s" s="2">
+        <v>189</v>
+      </c>
       <c r="O25" t="s" s="2">
         <v>41</v>
       </c>
@@ -3679,7 +3490,7 @@
         <v>41</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>39</v>
@@ -3694,15 +3505,15 @@
         <v>41</v>
       </c>
       <c r="AJ25" t="s" s="2">
-        <v>186</v>
+        <v>191</v>
       </c>
       <c r="AK25" t="s" s="2">
         <v>41</v>
       </c>
     </row>
-    <row r="26" hidden="true">
+    <row r="26">
       <c r="A26" t="s" s="2">
-        <v>187</v>
+        <v>192</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
@@ -3710,13 +3521,13 @@
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F26" t="s" s="2">
         <v>47</v>
       </c>
       <c r="G26" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="H26" t="s" s="2">
         <v>41</v>
@@ -3725,18 +3536,20 @@
         <v>48</v>
       </c>
       <c r="J26" t="s" s="2">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>191</v>
-      </c>
-      <c r="N26" s="2"/>
+        <v>196</v>
+      </c>
+      <c r="N26" t="s" s="2">
+        <v>197</v>
+      </c>
       <c r="O26" t="s" s="2">
         <v>41</v>
       </c>
@@ -3799,15 +3612,15 @@
         <v>41</v>
       </c>
       <c r="AJ26" t="s" s="2">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>41</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -3815,7 +3628,7 @@
       </c>
       <c r="D27" s="2"/>
       <c r="E27" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="F27" t="s" s="2">
         <v>47</v>
@@ -3824,25 +3637,23 @@
         <v>41</v>
       </c>
       <c r="H27" t="s" s="2">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I27" t="s" s="2">
         <v>48</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>157</v>
+        <v>201</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>196</v>
-      </c>
-      <c r="M27" t="s" s="2">
-        <v>197</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="M27" s="2"/>
       <c r="N27" t="s" s="2">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>41</v>
@@ -3867,34 +3678,34 @@
         <v>41</v>
       </c>
       <c r="W27" t="s" s="2">
-        <v>199</v>
+        <v>41</v>
       </c>
       <c r="X27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Y27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="Z27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AA27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AB27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AC27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AD27" t="s" s="2">
+        <v>41</v>
+      </c>
+      <c r="AE27" t="s" s="2">
         <v>200</v>
       </c>
-      <c r="Y27" t="s" s="2">
-        <v>201</v>
-      </c>
-      <c r="Z27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD27" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE27" t="s" s="2">
-        <v>194</v>
-      </c>
       <c r="AF27" t="s" s="2">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>47</v>
@@ -3906,15 +3717,15 @@
         <v>41</v>
       </c>
       <c r="AJ27" t="s" s="2">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>203</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -3934,19 +3745,21 @@
         <v>41</v>
       </c>
       <c r="I28" t="s" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="J28" t="s" s="2">
-        <v>121</v>
+        <v>208</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>122</v>
+        <v>209</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>123</v>
+        <v>210</v>
       </c>
       <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="N28" t="s" s="2">
+        <v>211</v>
+      </c>
       <c r="O28" t="s" s="2">
         <v>41</v>
       </c>
@@ -3994,7 +3807,7 @@
         <v>41</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>124</v>
+        <v>207</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>39</v>
@@ -4009,1387 +3822,14 @@
         <v>41</v>
       </c>
       <c r="AJ28" t="s" s="2">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" hidden="true">
-      <c r="A29" t="s" s="2">
-        <v>205</v>
-      </c>
-      <c r="B29" s="2"/>
-      <c r="C29" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="D29" s="2"/>
-      <c r="E29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F29" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J29" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="K29" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="L29" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="M29" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="N29" s="2"/>
-      <c r="O29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P29" s="2"/>
-      <c r="Q29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA29" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="AB29" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="AC29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD29" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AE29" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="AF29" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG29" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI29" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ29" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="AK29" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="s" s="2">
-        <v>206</v>
-      </c>
-      <c r="B30" s="2"/>
-      <c r="C30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D30" s="2"/>
-      <c r="E30" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="F30" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G30" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="H30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I30" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J30" t="s" s="2">
-        <v>207</v>
-      </c>
-      <c r="K30" t="s" s="2">
-        <v>208</v>
-      </c>
-      <c r="L30" t="s" s="2">
-        <v>209</v>
-      </c>
-      <c r="M30" t="s" s="2">
-        <v>210</v>
-      </c>
-      <c r="N30" t="s" s="2">
-        <v>211</v>
-      </c>
-      <c r="O30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P30" s="2"/>
-      <c r="Q30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE30" t="s" s="2">
-        <v>212</v>
-      </c>
-      <c r="AF30" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG30" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI30" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ30" t="s" s="2">
         <v>213</v>
-      </c>
-      <c r="AK30" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" hidden="true">
-      <c r="A31" t="s" s="2">
-        <v>214</v>
-      </c>
-      <c r="B31" s="2"/>
-      <c r="C31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D31" s="2"/>
-      <c r="E31" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F31" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J31" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="K31" t="s" s="2">
-        <v>122</v>
-      </c>
-      <c r="L31" t="s" s="2">
-        <v>123</v>
-      </c>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
-      <c r="O31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P31" s="2"/>
-      <c r="Q31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE31" t="s" s="2">
-        <v>124</v>
-      </c>
-      <c r="AF31" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG31" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI31" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ31" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="AK31" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="32" hidden="true">
-      <c r="A32" t="s" s="2">
-        <v>215</v>
-      </c>
-      <c r="B32" s="2"/>
-      <c r="C32" t="s" s="2">
-        <v>108</v>
-      </c>
-      <c r="D32" s="2"/>
-      <c r="E32" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F32" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="G32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="J32" t="s" s="2">
-        <v>91</v>
-      </c>
-      <c r="K32" t="s" s="2">
-        <v>127</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>128</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>111</v>
-      </c>
-      <c r="N32" s="2"/>
-      <c r="O32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P32" s="2"/>
-      <c r="Q32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA32" t="s" s="2">
-        <v>94</v>
-      </c>
-      <c r="AB32" t="s" s="2">
-        <v>129</v>
-      </c>
-      <c r="AC32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD32" t="s" s="2">
-        <v>95</v>
-      </c>
-      <c r="AE32" t="s" s="2">
-        <v>130</v>
-      </c>
-      <c r="AF32" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG32" t="s" s="2">
-        <v>40</v>
-      </c>
-      <c r="AH32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI32" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ32" t="s" s="2">
-        <v>125</v>
-      </c>
-      <c r="AK32" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="33" hidden="true">
-      <c r="A33" t="s" s="2">
-        <v>216</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D33" s="2"/>
-      <c r="E33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F33" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I33" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J33" t="s" s="2">
-        <v>60</v>
-      </c>
-      <c r="K33" t="s" s="2">
-        <v>217</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>218</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>219</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>220</v>
-      </c>
-      <c r="O33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P33" s="2"/>
-      <c r="Q33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE33" t="s" s="2">
-        <v>221</v>
-      </c>
-      <c r="AF33" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG33" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI33" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ33" t="s" s="2">
-        <v>222</v>
-      </c>
-      <c r="AK33" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="34" hidden="true">
-      <c r="A34" t="s" s="2">
-        <v>223</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D34" s="2"/>
-      <c r="E34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F34" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I34" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J34" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="K34" t="s" s="2">
-        <v>224</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>225</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>226</v>
-      </c>
-      <c r="N34" s="2"/>
-      <c r="O34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P34" s="2"/>
-      <c r="Q34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE34" t="s" s="2">
-        <v>227</v>
-      </c>
-      <c r="AF34" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG34" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI34" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ34" t="s" s="2">
-        <v>228</v>
-      </c>
-      <c r="AK34" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="s" s="2">
-        <v>229</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D35" s="2"/>
-      <c r="E35" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="F35" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G35" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="H35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I35" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J35" t="s" s="2">
-        <v>66</v>
-      </c>
-      <c r="K35" t="s" s="2">
-        <v>230</v>
-      </c>
-      <c r="L35" t="s" s="2">
-        <v>231</v>
-      </c>
-      <c r="M35" s="2"/>
-      <c r="N35" t="s" s="2">
-        <v>232</v>
-      </c>
-      <c r="O35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P35" s="2"/>
-      <c r="Q35" t="s" s="2">
-        <v>233</v>
-      </c>
-      <c r="R35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE35" t="s" s="2">
-        <v>234</v>
-      </c>
-      <c r="AF35" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG35" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI35" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ35" t="s" s="2">
-        <v>202</v>
-      </c>
-      <c r="AK35" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" hidden="true">
-      <c r="A36" t="s" s="2">
-        <v>235</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D36" s="2"/>
-      <c r="E36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F36" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I36" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J36" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="K36" t="s" s="2">
-        <v>236</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>237</v>
-      </c>
-      <c r="M36" s="2"/>
-      <c r="N36" t="s" s="2">
-        <v>238</v>
-      </c>
-      <c r="O36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P36" s="2"/>
-      <c r="Q36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE36" t="s" s="2">
-        <v>239</v>
-      </c>
-      <c r="AF36" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG36" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI36" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ36" t="s" s="2">
-        <v>240</v>
-      </c>
-      <c r="AK36" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="37" hidden="true">
-      <c r="A37" t="s" s="2">
-        <v>241</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F37" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I37" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J37" t="s" s="2">
-        <v>242</v>
-      </c>
-      <c r="K37" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>246</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P37" s="2"/>
-      <c r="Q37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE37" t="s" s="2">
-        <v>247</v>
-      </c>
-      <c r="AF37" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG37" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI37" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ37" t="s" s="2">
-        <v>248</v>
-      </c>
-      <c r="AK37" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" hidden="true">
-      <c r="A38" t="s" s="2">
-        <v>249</v>
-      </c>
-      <c r="B38" s="2"/>
-      <c r="C38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D38" s="2"/>
-      <c r="E38" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F38" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I38" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J38" t="s" s="2">
-        <v>121</v>
-      </c>
-      <c r="K38" t="s" s="2">
-        <v>250</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P38" s="2"/>
-      <c r="Q38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE38" t="s" s="2">
-        <v>254</v>
-      </c>
-      <c r="AF38" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG38" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI38" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ38" t="s" s="2">
-        <v>255</v>
-      </c>
-      <c r="AK38" t="s" s="2">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="B39" s="2"/>
-      <c r="C39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D39" s="2"/>
-      <c r="E39" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="F39" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G39" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="H39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I39" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J39" t="s" s="2">
-        <v>257</v>
-      </c>
-      <c r="K39" t="s" s="2">
-        <v>258</v>
-      </c>
-      <c r="L39" t="s" s="2">
-        <v>259</v>
-      </c>
-      <c r="M39" t="s" s="2">
-        <v>260</v>
-      </c>
-      <c r="N39" t="s" s="2">
-        <v>261</v>
-      </c>
-      <c r="O39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P39" s="2"/>
-      <c r="Q39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE39" t="s" s="2">
-        <v>256</v>
-      </c>
-      <c r="AF39" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG39" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI39" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ39" t="s" s="2">
-        <v>262</v>
-      </c>
-      <c r="AK39" t="s" s="2">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="40" hidden="true">
-      <c r="A40" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="B40" s="2"/>
-      <c r="C40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D40" s="2"/>
-      <c r="E40" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F40" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I40" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J40" t="s" s="2">
-        <v>265</v>
-      </c>
-      <c r="K40" t="s" s="2">
-        <v>266</v>
-      </c>
-      <c r="L40" t="s" s="2">
-        <v>267</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" t="s" s="2">
-        <v>268</v>
-      </c>
-      <c r="O40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P40" s="2"/>
-      <c r="Q40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE40" t="s" s="2">
-        <v>264</v>
-      </c>
-      <c r="AF40" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG40" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI40" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ40" t="s" s="2">
-        <v>269</v>
-      </c>
-      <c r="AK40" t="s" s="2">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="41" hidden="true">
-      <c r="A41" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="B41" s="2"/>
-      <c r="C41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="D41" s="2"/>
-      <c r="E41" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="F41" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="G41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="H41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="I41" t="s" s="2">
-        <v>48</v>
-      </c>
-      <c r="J41" t="s" s="2">
-        <v>272</v>
-      </c>
-      <c r="K41" t="s" s="2">
-        <v>273</v>
-      </c>
-      <c r="L41" t="s" s="2">
-        <v>274</v>
-      </c>
-      <c r="M41" s="2"/>
-      <c r="N41" t="s" s="2">
-        <v>275</v>
-      </c>
-      <c r="O41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="P41" s="2"/>
-      <c r="Q41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="R41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="S41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="T41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="U41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="V41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="W41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="X41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Y41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="Z41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AA41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AB41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AC41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AD41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AE41" t="s" s="2">
-        <v>271</v>
-      </c>
-      <c r="AF41" t="s" s="2">
-        <v>39</v>
-      </c>
-      <c r="AG41" t="s" s="2">
-        <v>47</v>
-      </c>
-      <c r="AH41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AI41" t="s" s="2">
-        <v>41</v>
-      </c>
-      <c r="AJ41" t="s" s="2">
-        <v>276</v>
-      </c>
-      <c r="AK41" t="s" s="2">
-        <v>277</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AK41">
+  <autoFilter ref="A1:AK28">
     <filterColumn colId="6">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
@@ -5399,7 +3839,7 @@
       <filters blank="true"/>
     </filterColumn>
   </autoFilter>
-  <conditionalFormatting sqref="A2:AI40">
+  <conditionalFormatting sqref="A2:AI27">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>$G2&lt;&gt;"Y"</formula>
     </cfRule>

</xml_diff>